<commit_message>
Updated mistakes methodology section
</commit_message>
<xml_diff>
--- a/Data/method_summaryData.xlsx
+++ b/Data/method_summaryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiagopardo/Documents/GitHub/LAC-Reports/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73E658D-04A1-5645-AFE5-63DD6A87EBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9314C-EB72-604E-B743-0D49ECC8B04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling_Frame" sheetId="5" r:id="rId1"/>
@@ -634,9 +634,6 @@
     <t xml:space="preserve">The supervisory team directly oversaw approximately 9% of all interviews in the field. During data processing, 356 interviews (approximately 35% of the sample) were selected for audio review by the central office and 86 interviews (approximately 8% of the sample) were backchecked via telephone. Interviews averaged 38 minutes in length. </t>
   </si>
   <si>
-    <t xml:space="preserve">Regions and cities were selected to achieve a nationally representative sample of the country. In city districts, neighborhoods served as the primary sampling unit and were randomly selected based on relative population sizes and the socioeconomic level distribution within each city. Within each neighborhood, blocks were selected as enumeration areas using simple random sampling. In rural areas, veredas, or municipalities, served as the primary sampling unit and were randomly selected based on relative population sizes and the socioeconomic level distribution within each area. Within each vereda, zones were selected as enumeration areas using simple random sampling. Within each enumeration area, survey administrators performed a systematic random route to sample households and used a Kish grid to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.  </t>
-  </si>
-  <si>
     <t>Face-to-Face</t>
   </si>
   <si>
@@ -1205,6 +1202,9 @@
   </si>
   <si>
     <t>Thirty-eight percent (38%) of the interviews took place in Paramaribo, followed by 33% in Wanica, 7% in Nickerie, and the remaining 22% in other regions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regions and cities were selected to achieve a nationally representative sample of the country. In city districts, neighborhoods served as the primary sampling unit and were randomly selected based on relative population sizes and the socioeconomic level distribution within each city. Within each neighborhood, blocks were selected as enumeration areas using simple random sampling. In rural areas, &lt;i&gt; veredas &lt;/i&gt;, or municipalities, served as the primary sampling unit and were randomly selected based on relative population sizes and the socioeconomic level distribution within each area. Within each vereda, zones were selected as enumeration areas using simple random sampling. Within each enumeration area, survey administrators performed a systematic random route to sample households and used a Kish grid to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.  </t>
   </si>
 </sst>
 </file>
@@ -1815,11 +1815,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A370D2-6729-6642-9050-0182FD4A6CB8}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -1994,7 +1994,7 @@
         <v>123</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>196</v>
+        <v>385</v>
       </c>
       <c r="P3" s="22" t="s">
         <v>184</v>
@@ -2150,40 +2150,40 @@
         <v>16</v>
       </c>
       <c r="H6" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="K6" s="21" t="s">
         <v>214</v>
-      </c>
-      <c r="K6" s="21" t="s">
-        <v>215</v>
       </c>
       <c r="L6" s="13" t="s">
         <v>117</v>
       </c>
       <c r="M6" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="N6" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="O6" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="P6" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="Q6" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="R6" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="R6" s="21" t="s">
+      <c r="S6" s="13" t="s">
         <v>221</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="126" customHeight="1">
@@ -2209,40 +2209,40 @@
         <v>16</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I7" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="K7" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="L7" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="M7" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="N7" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="O7" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="P7" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="P7" s="21" t="s">
+      <c r="Q7" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="R7" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="S7" s="13" t="s">
         <v>232</v>
-      </c>
-      <c r="S7" s="13" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="126" customHeight="1">
@@ -2259,49 +2259,49 @@
         <v>1000</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F8" s="13">
         <v>2021</v>
       </c>
       <c r="G8" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="I8" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>236</v>
       </c>
       <c r="J8" s="21" t="s">
         <v>190</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L8" s="13" t="s">
         <v>117</v>
       </c>
       <c r="M8" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="N8" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="O8" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="P8" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="Q8" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="R8" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="R8" s="21" t="s">
+      <c r="S8" s="13" t="s">
         <v>243</v>
-      </c>
-      <c r="S8" s="13" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="126" customHeight="1">
@@ -2318,7 +2318,7 @@
         <v>500</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F9" s="21">
         <v>2022</v>
@@ -2327,40 +2327,40 @@
         <v>20</v>
       </c>
       <c r="H9" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="I9" s="21" t="s">
         <v>278</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>279</v>
       </c>
       <c r="J9" s="21" t="s">
         <v>157</v>
       </c>
       <c r="K9" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="L9" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="M9" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="N9" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="O9" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="P9" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="Q9" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="R9" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="R9" s="21" t="s">
+      <c r="S9" s="21" t="s">
         <v>287</v>
-      </c>
-      <c r="S9" s="21" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="126" customHeight="1">
@@ -2386,40 +2386,40 @@
         <v>2022</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I10" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="K10" s="21" t="s">
         <v>290</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>291</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>117</v>
       </c>
       <c r="M10" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="N10" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="O10" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="P10" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="Q10" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="R10" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="R10" s="21" t="s">
+      <c r="S10" s="21" t="s">
         <v>297</v>
-      </c>
-      <c r="S10" s="21" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="126" customHeight="1">
@@ -2442,43 +2442,43 @@
         <v>2022</v>
       </c>
       <c r="G11" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="I11" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="I11" s="21" t="s">
+      <c r="J11" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="K11" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="J11" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="K11" s="21" t="s">
+      <c r="L11" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="M11" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="L11" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="M11" s="21" t="s">
+      <c r="N11" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="O11" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="P11" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="P11" s="21" t="s">
+      <c r="Q11" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="Q11" s="21" t="s">
+      <c r="R11" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="R11" s="21" t="s">
+      <c r="S11" s="21" t="s">
         <v>307</v>
-      </c>
-      <c r="S11" s="21" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="126" customHeight="1">
@@ -2504,40 +2504,40 @@
         <v>2022</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I12" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="K12" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="J12" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="K12" s="21" t="s">
+      <c r="L12" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="M12" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="N12" s="21" t="s">
         <v>312</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="O12" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="O12" s="21" t="s">
+      <c r="P12" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="P12" s="21" t="s">
+      <c r="Q12" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="Q12" s="21" t="s">
+      <c r="R12" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="R12" s="21" t="s">
+      <c r="S12" s="21" t="s">
         <v>317</v>
-      </c>
-      <c r="S12" s="21" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="126" customHeight="1">
@@ -2563,40 +2563,40 @@
         <v>2022</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I13" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="K13" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="J13" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="K13" s="21" t="s">
+      <c r="L13" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="M13" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="L13" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="M13" s="21" t="s">
+      <c r="N13" s="21" t="s">
         <v>321</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="O13" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="O13" s="21" t="s">
+      <c r="P13" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="Q13" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="Q13" s="21" t="s">
+      <c r="R13" s="21" t="s">
         <v>325</v>
       </c>
-      <c r="R13" s="21" t="s">
+      <c r="S13" s="21" t="s">
         <v>326</v>
-      </c>
-      <c r="S13" s="21" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="126" customHeight="1">
@@ -2622,40 +2622,40 @@
         <v>2022</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I14" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="J14" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="K14" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="L14" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="M14" s="21" t="s">
         <v>331</v>
       </c>
-      <c r="M14" s="21" t="s">
+      <c r="N14" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="O14" s="21" t="s">
         <v>333</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="P14" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="Q14" s="21" t="s">
         <v>335</v>
       </c>
-      <c r="Q14" s="21" t="s">
+      <c r="R14" s="21" t="s">
         <v>336</v>
       </c>
-      <c r="R14" s="21" t="s">
+      <c r="S14" s="21" t="s">
         <v>337</v>
-      </c>
-      <c r="S14" s="21" t="s">
-        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -2731,7 +2731,7 @@
         <v>29</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2745,7 +2745,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2759,7 +2759,7 @@
         <v>32</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E4" s="11"/>
     </row>
@@ -2789,7 +2789,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2800,10 +2800,10 @@
         <v>28</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="31" t="s">
         <v>205</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2817,7 +2817,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E8" s="11"/>
     </row>
@@ -2847,7 +2847,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2861,7 +2861,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2875,7 +2875,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E12" s="11"/>
     </row>
@@ -2887,10 +2887,10 @@
         <v>101</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>245</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>246</v>
       </c>
       <c r="E13" s="11"/>
     </row>
@@ -2902,7 +2902,7 @@
         <v>107</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2913,7 +2913,7 @@
         <v>101</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D15" s="13">
         <v>17</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>107</v>
@@ -2930,13 +2930,13 @@
         <v>32</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>101</v>
@@ -2945,7 +2945,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E17" s="11"/>
     </row>
@@ -2971,7 +2971,7 @@
         <v>101</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D19" s="13">
         <v>31</v>
@@ -2988,7 +2988,7 @@
         <v>32</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E20" s="11"/>
     </row>
@@ -3000,7 +3000,7 @@
         <v>28</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D21" s="11">
         <v>26</v>
@@ -3018,7 +3018,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3029,7 +3029,7 @@
         <v>101</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D23" s="13">
         <v>10</v>
@@ -3046,7 +3046,7 @@
         <v>32</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E24" s="11"/>
     </row>
@@ -3058,7 +3058,7 @@
         <v>101</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D25" s="11">
         <v>15</v>
@@ -3076,7 +3076,7 @@
         <v>32</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3087,7 +3087,7 @@
         <v>101</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D27" s="13">
         <v>28</v>
@@ -3103,7 +3103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B7FB5B-1ADA-344B-BEC0-179A66FAE9C7}">
   <dimension ref="A1:H262"/>
   <sheetViews>
-    <sheetView topLeftCell="A229" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F229" sqref="F229"/>
     </sheetView>
   </sheetViews>
@@ -3279,7 +3279,7 @@
         <v>142</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D11" s="16"/>
       <c r="G11" s="37"/>
@@ -3522,7 +3522,7 @@
         <v>142</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D28" s="12"/>
     </row>
@@ -3745,7 +3745,7 @@
         <v>142</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D44" s="16"/>
     </row>
@@ -4010,7 +4010,7 @@
         <v>142</v>
       </c>
       <c r="C63" s="36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D63" s="12"/>
     </row>
@@ -4207,7 +4207,7 @@
         <v>3</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D77" s="13">
         <v>0.39500000000000002</v>
@@ -4221,7 +4221,7 @@
         <v>3</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D78" s="13">
         <v>0.1</v>
@@ -4235,7 +4235,7 @@
         <v>3</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D79" s="13">
         <v>0.107</v>
@@ -4249,7 +4249,7 @@
         <v>3</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D80" s="13">
         <v>0.2</v>
@@ -4263,7 +4263,7 @@
         <v>3</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D81" s="13">
         <v>0.11</v>
@@ -4277,7 +4277,7 @@
         <v>3</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D82" s="13">
         <v>9.1999999999999998E-2</v>
@@ -4291,7 +4291,7 @@
         <v>142</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -4484,7 +4484,7 @@
         <v>3</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D97" s="11">
         <v>0.54</v>
@@ -4498,7 +4498,7 @@
         <v>3</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D98" s="11">
         <v>0.21</v>
@@ -4540,7 +4540,7 @@
         <v>3</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D101" s="11">
         <v>0.03</v>
@@ -4554,7 +4554,7 @@
         <v>142</v>
       </c>
       <c r="C102" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D102" s="11"/>
     </row>
@@ -4748,7 +4748,7 @@
         <v>3</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D116" s="13">
         <v>0.115</v>
@@ -4762,7 +4762,7 @@
         <v>3</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D117" s="13">
         <v>2.4E-2</v>
@@ -4776,7 +4776,7 @@
         <v>3</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D118" s="13">
         <v>7.0999999999999994E-2</v>
@@ -4790,7 +4790,7 @@
         <v>3</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D119" s="13">
         <v>1.2E-2</v>
@@ -4804,7 +4804,7 @@
         <v>3</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D120" s="13">
         <v>7.8E-2</v>
@@ -4818,7 +4818,7 @@
         <v>3</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D121" s="13">
         <v>2.6000000000000002E-2</v>
@@ -4832,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D122" s="13">
         <v>3.2000000000000001E-2</v>
@@ -4860,7 +4860,7 @@
         <v>3</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D124" s="13">
         <v>3.5000000000000003E-2</v>
@@ -4874,7 +4874,7 @@
         <v>3</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D125" s="13">
         <v>4.2999999999999997E-2</v>
@@ -4888,7 +4888,7 @@
         <v>3</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D126" s="13">
         <v>3.1E-2</v>
@@ -4902,7 +4902,7 @@
         <v>3</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D127" s="13">
         <v>8.5000000000000006E-2</v>
@@ -4916,7 +4916,7 @@
         <v>3</v>
       </c>
       <c r="C128" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D128" s="13">
         <v>1.7999999999999999E-2</v>
@@ -4930,7 +4930,7 @@
         <v>3</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D129" s="13">
         <v>1.2E-2</v>
@@ -4944,7 +4944,7 @@
         <v>3</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D130" s="13">
         <v>3.5999999999999997E-2</v>
@@ -4958,7 +4958,7 @@
         <v>3</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D131" s="13">
         <v>1.7999999999999999E-2</v>
@@ -4972,7 +4972,7 @@
         <v>3</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D132" s="13">
         <v>6.0999999999999999E-2</v>
@@ -4986,7 +4986,7 @@
         <v>142</v>
       </c>
       <c r="C133" s="21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -5173,13 +5173,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B147" s="11" t="s">
         <v>96</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D147" s="11">
         <v>0.78</v>
@@ -5187,13 +5187,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B148" s="11" t="s">
         <v>98</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D148" s="11">
         <v>0.16</v>
@@ -5201,13 +5201,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B149" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D149" s="11">
         <v>0.06</v>
@@ -5215,19 +5215,19 @@
     </row>
     <row r="150" spans="1:4" ht="48">
       <c r="A150" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B150" s="11" t="s">
         <v>142</v>
       </c>
       <c r="C150" s="38" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D150" s="11"/>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B151" s="11" t="s">
         <v>52</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B152" s="11" t="s">
         <v>52</v>
@@ -5255,7 +5255,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B153" s="11" t="s">
         <v>55</v>
@@ -5269,7 +5269,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B154" s="11" t="s">
         <v>55</v>
@@ -5283,7 +5283,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B155" s="11" t="s">
         <v>58</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B156" s="11" t="s">
         <v>58</v>
@@ -5311,7 +5311,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B157" s="11" t="s">
         <v>58</v>
@@ -5325,7 +5325,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B158" s="11" t="s">
         <v>58</v>
@@ -5339,7 +5339,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B159" s="11" t="s">
         <v>58</v>
@@ -5353,7 +5353,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B160" s="11" t="s">
         <v>58</v>
@@ -5367,7 +5367,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B161" s="11" t="s">
         <v>58</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B162" s="11" t="s">
         <v>58</v>
@@ -5395,7 +5395,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B163" s="11" t="s">
         <v>58</v>
@@ -5412,10 +5412,10 @@
         <v>162</v>
       </c>
       <c r="B164" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="C164" s="13" t="s">
         <v>346</v>
-      </c>
-      <c r="C164" s="13" t="s">
-        <v>347</v>
       </c>
       <c r="D164" s="13">
         <v>0.37</v>
@@ -5426,10 +5426,10 @@
         <v>162</v>
       </c>
       <c r="B165" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C165" s="13" t="s">
         <v>348</v>
-      </c>
-      <c r="C165" s="13" t="s">
-        <v>349</v>
       </c>
       <c r="D165" s="13">
         <v>0.16</v>
@@ -5440,10 +5440,10 @@
         <v>162</v>
       </c>
       <c r="B166" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C166" s="13" t="s">
         <v>350</v>
-      </c>
-      <c r="C166" s="13" t="s">
-        <v>351</v>
       </c>
       <c r="D166" s="13">
         <v>0.1</v>
@@ -5454,10 +5454,10 @@
         <v>162</v>
       </c>
       <c r="B167" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="C167" s="13" t="s">
         <v>352</v>
-      </c>
-      <c r="C167" s="13" t="s">
-        <v>353</v>
       </c>
       <c r="D167" s="13">
         <v>0.08</v>
@@ -5468,10 +5468,10 @@
         <v>162</v>
       </c>
       <c r="B168" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="C168" s="13" t="s">
         <v>354</v>
-      </c>
-      <c r="C168" s="13" t="s">
-        <v>355</v>
       </c>
       <c r="D168" s="13">
         <v>0.06</v>
@@ -5482,10 +5482,10 @@
         <v>162</v>
       </c>
       <c r="B169" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="C169" s="13" t="s">
         <v>356</v>
-      </c>
-      <c r="C169" s="13" t="s">
-        <v>357</v>
       </c>
       <c r="D169" s="13">
         <v>0.06</v>
@@ -5496,10 +5496,10 @@
         <v>162</v>
       </c>
       <c r="B170" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="C170" s="13" t="s">
         <v>358</v>
-      </c>
-      <c r="C170" s="13" t="s">
-        <v>359</v>
       </c>
       <c r="D170" s="13">
         <v>0.06</v>
@@ -5510,10 +5510,10 @@
         <v>162</v>
       </c>
       <c r="B171" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="C171" s="13" t="s">
         <v>360</v>
-      </c>
-      <c r="C171" s="13" t="s">
-        <v>361</v>
       </c>
       <c r="D171" s="13">
         <v>0.04</v>
@@ -5524,10 +5524,10 @@
         <v>162</v>
       </c>
       <c r="B172" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="C172" s="13" t="s">
         <v>362</v>
-      </c>
-      <c r="C172" s="13" t="s">
-        <v>363</v>
       </c>
       <c r="D172" s="13">
         <v>0.04</v>
@@ -5538,10 +5538,10 @@
         <v>162</v>
       </c>
       <c r="B173" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="C173" s="13" t="s">
         <v>364</v>
-      </c>
-      <c r="C173" s="13" t="s">
-        <v>365</v>
       </c>
       <c r="D173" s="13">
         <v>3.1E-2</v>
@@ -5555,7 +5555,7 @@
         <v>142</v>
       </c>
       <c r="C174" s="21" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -5748,7 +5748,7 @@
         <v>96</v>
       </c>
       <c r="C188" s="11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D188" s="11">
         <v>0.73</v>
@@ -5762,7 +5762,7 @@
         <v>98</v>
       </c>
       <c r="C189" s="11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D189" s="11">
         <v>0.14199999999999999</v>
@@ -5773,10 +5773,10 @@
         <v>163</v>
       </c>
       <c r="B190" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C190" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D190" s="11">
         <v>0.128</v>
@@ -5790,7 +5790,7 @@
         <v>142</v>
       </c>
       <c r="C191" s="38" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D191" s="11"/>
     </row>
@@ -5984,7 +5984,7 @@
         <v>96</v>
       </c>
       <c r="C205" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D205" s="13">
         <v>0.36899999999999999</v>
@@ -6040,7 +6040,7 @@
         <v>142</v>
       </c>
       <c r="C209" s="21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -6230,10 +6230,10 @@
         <v>165</v>
       </c>
       <c r="B223" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C223" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D223" s="11">
         <v>0.45800000000000002</v>
@@ -6244,10 +6244,10 @@
         <v>165</v>
       </c>
       <c r="B224" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D224" s="11">
         <v>0.31</v>
@@ -6258,10 +6258,10 @@
         <v>165</v>
       </c>
       <c r="B225" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C225" s="11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D225" s="11">
         <v>0.23</v>
@@ -6275,7 +6275,7 @@
         <v>142</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D226" s="11"/>
     </row>
@@ -6469,7 +6469,7 @@
         <v>96</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D240" s="13">
         <v>0.38</v>
@@ -6483,7 +6483,7 @@
         <v>98</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D241" s="13">
         <v>0.33</v>
@@ -6497,7 +6497,7 @@
         <v>97</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D242" s="13">
         <v>7.0000000000000007E-2</v>
@@ -6511,7 +6511,7 @@
         <v>99</v>
       </c>
       <c r="C243" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D243" s="13">
         <v>0.06</v>
@@ -6525,7 +6525,7 @@
         <v>100</v>
       </c>
       <c r="C244" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D244" s="13">
         <v>0.05</v>
@@ -6539,7 +6539,7 @@
         <v>102</v>
       </c>
       <c r="C245" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D245" s="13">
         <v>0.04</v>
@@ -6553,7 +6553,7 @@
         <v>103</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D246" s="13">
         <v>0.04</v>
@@ -6567,7 +6567,7 @@
         <v>104</v>
       </c>
       <c r="C247" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D247" s="13">
         <v>0.03</v>
@@ -6581,7 +6581,7 @@
         <v>105</v>
       </c>
       <c r="C248" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D248" s="13">
         <v>0.01</v>
@@ -6595,7 +6595,7 @@
         <v>142</v>
       </c>
       <c r="C249" s="21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -6789,7 +6789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F8BEAD-D473-7B4F-A0F1-FD90B83F8C12}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -7007,7 +7007,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2" s="29">
         <v>1000</v>
@@ -7024,7 +7024,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E3" s="29">
         <v>1000</v>
@@ -7041,7 +7041,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="29">
         <v>1005</v>
@@ -7058,7 +7058,7 @@
         <v>146</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="29">
         <v>1029</v>
@@ -7075,7 +7075,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" s="28">
         <v>759</v>
@@ -7092,7 +7092,7 @@
         <v>149</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="29">
         <v>1109</v>
@@ -7106,10 +7106,10 @@
         <v>145</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="29">
         <v>1000</v>
@@ -7126,7 +7126,7 @@
         <v>152</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="28">
         <v>500</v>
@@ -7143,7 +7143,7 @@
         <v>152</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="28">
         <v>500</v>
@@ -7160,7 +7160,7 @@
         <v>152</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="28">
         <v>500</v>
@@ -7177,7 +7177,7 @@
         <v>152</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E12" s="28">
         <v>500</v>
@@ -7194,7 +7194,7 @@
         <v>152</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E13" s="28">
         <v>499</v>
@@ -7211,7 +7211,7 @@
         <v>152</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E14" s="28">
         <v>500</v>
@@ -7228,7 +7228,7 @@
         <v>152</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E15" s="28">
         <v>500</v>
@@ -7245,7 +7245,7 @@
         <v>160</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E16" s="29">
         <v>1001</v>
@@ -7262,7 +7262,7 @@
         <v>152</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E17" s="28">
         <v>500</v>
@@ -7279,7 +7279,7 @@
         <v>160</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E18" s="29">
         <v>1002</v>
@@ -7296,7 +7296,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E19" s="28">
         <v>500</v>
@@ -7313,7 +7313,7 @@
         <v>160</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E20" s="28">
         <v>507</v>
@@ -7330,7 +7330,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E21" s="28">
         <v>531</v>
@@ -7347,7 +7347,7 @@
         <v>167</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E22" s="28">
         <v>522</v>
@@ -7364,7 +7364,7 @@
         <v>160</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E23" s="29">
         <v>1500</v>
@@ -7381,7 +7381,7 @@
         <v>160</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E24" s="29">
         <v>1002</v>
@@ -7398,7 +7398,7 @@
         <v>160</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E25" s="29">
         <v>2010</v>
@@ -7415,7 +7415,7 @@
         <v>172</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E26" s="29">
         <v>2002</v>
@@ -7432,7 +7432,7 @@
         <v>172</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E27" s="29">
         <v>2000</v>
@@ -7440,7 +7440,7 @@
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1" thickBot="1">
       <c r="A28" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>145</v>
@@ -7449,7 +7449,7 @@
         <v>160</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E28" s="29">
         <v>1014</v>
@@ -7466,7 +7466,7 @@
         <v>160</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E29" s="29">
         <v>2023</v>
@@ -8706,15 +8706,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
@@ -8723,6 +8714,15 @@
     <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8969,14 +8969,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -8989,6 +8981,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Changes in methodology excel
</commit_message>
<xml_diff>
--- a/Data/method_summaryData.xlsx
+++ b/Data/method_summaryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiagopardo/Documents/GitHub/LAC-Reports/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086020BD-301C-6A4B-8658-102CCB7257E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D84A917-4440-F24D-B88C-BDA3822885E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16060" windowHeight="18000" activeTab="3" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling_Frame" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="388">
   <si>
     <t>Sample Size</t>
   </si>
@@ -1821,7 +1821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A370D2-6729-6642-9050-0182FD4A6CB8}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6793,10 +6793,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F8BEAD-D473-7B4F-A0F1-FD90B83F8C12}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6965,6 +6965,23 @@
       </c>
       <c r="C8">
         <v>3500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9">
+        <v>445</v>
+      </c>
+      <c r="C9">
+        <v>284</v>
+      </c>
+      <c r="D9">
+        <v>73</v>
+      </c>
+      <c r="E9">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -8712,26 +8729,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b17f52af6646b5583120346a68295973">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95a1201d1da507c70fe2596948b34472" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -8974,32 +8971,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39BE83E1-4A56-468A-AE3B-AA02AC75EB69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9016,4 +9008,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Method Summary Data Updated
</commit_message>
<xml_diff>
--- a/Data/method_summaryData.xlsx
+++ b/Data/method_summaryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiagopardo/Documents/GitHub/LAC-Reports/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C4DE6-8553-A945-8FE2-4C49D197FC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EB62E5-0DA3-BD45-A4D2-D6EBDF19F9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16880" yWindow="500" windowWidth="11920" windowHeight="15700" activeTab="3" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling_Frame" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="392">
   <si>
     <t>Sample Size</t>
   </si>
@@ -885,12 +885,6 @@
     <t>English</t>
   </si>
   <si>
-    <t xml:space="preserve">Most respondents (35%) identified themselves as White, followed by Mixed Race (35%), and Black (20%). </t>
-  </si>
-  <si>
-    <t>Most respondents (96%) reported that they had received at least a high school diploma or  vocational degree and the remaining 3% of respondents received up to a middle school diploma.</t>
-  </si>
-  <si>
     <t>Given The Bahamas’ population size, regions served as the primary sampling unit. Interviewers were assigned a starting point within each primary sampling unit and performed a systemic random route, while paying close attention to target quotas for gender, age, and income. Interviewers used a Kish grid to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.</t>
   </si>
   <si>
@@ -915,15 +909,6 @@
     <t>CID Gallup based the sampling frame on 2018 population figures from the National Statistics Office of Dominican Republic (ONE), acquiring a proportionally stratified sample by region, age, gender, socioeconomic status, and level of urbanization</t>
   </si>
   <si>
-    <t xml:space="preserve">More than one-quarter of all respondents (27%) identified themselves as Mestizo, followed by Mulatto (24%) and White (20%). </t>
-  </si>
-  <si>
-    <t>Most respondents (52%) reported that they had received up to a middle school diploma, and the remaining 48% of respondents received at least a high school diploma or vocational degree.</t>
-  </si>
-  <si>
-    <t>Regions, provinces, and municipalities were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Districts were then selected as the primary sampling unit using probability proportionate to size sampling. Within cities and towns, enumeration areas were selected at the cantón, or neighborhood, level via systematic random sampling based on the population of each area. Within the sampled segments, survey administrators performed a systematic random route to sample households and used the Last Birthday method to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.</t>
-  </si>
-  <si>
     <t>In total, 52 interviewers worked on this project, including 31 female interviewers. Enumerators worked in ten groups of five to six interviewers with one to two supervisors per group. Interviews were conducted in Spanish.</t>
   </si>
   <si>
@@ -936,30 +921,12 @@
     <t>The Bahamas, Guyana, Haiti, Jamaica, and Suriname</t>
   </si>
   <si>
-    <t>2018 / 2022</t>
-  </si>
-  <si>
-    <t>Guyanese individual</t>
-  </si>
-  <si>
     <t>StatMark Group based the sampling frame on 2012 population figures from the Bureau of Statistics of Guyana, acquiring a proportionally stratified sample by region, age, gender, socioeconomic status, and level of urbanization</t>
   </si>
   <si>
-    <t xml:space="preserve">Thirty percent (39%) of respondents identified themselves as Afro-Guyanese, followed by Mixed-Race (26%) and Indo-Guyanese (23%). </t>
-  </si>
-  <si>
-    <t>Most respondents (55%) reported that they had received at least a high school diploma or  vocational degree and the remaining 42% of respondents received up to a middle school diploma.</t>
-  </si>
-  <si>
-    <t>Regions and cities were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Within cities, neighborhoods were selected as primary sampling units using probability proportional to size sampling. Street blocks within the primary sampling units were selected at random, and each house within the selected segment was approached. Within the sampled segments, survey administrators performed a systematic random route to sample households and used a Kish grid to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.</t>
-  </si>
-  <si>
     <t>In total, 21 interviewers worked on this project, all of whom were female. Enumerators worked in five groups of three to five interviewers. Interviews were conducted in English.</t>
   </si>
   <si>
-    <t>The supervisory team directly oversaw or backchecked via telephone 150 interviews (approximately 30% of the total sample). Additional quality control measures included geo-fencing, audio quality checks, and checks for abnormal answer patterns. Interviews averaged 41 minutes in length and ranged from 21 to 108 minutes.</t>
-  </si>
-  <si>
     <t>Data for Guyana, The Bahamas, and Suriname was collected in 2016, 2018, and 2022. Data for the Dominican Republic was collected in 2013, 2016, 2018, and 2022. Data for Haiti was collected in 2021 and 2022. Data for Jamaica was collected in 2011, 2014, 2017, 2019, and 2022</t>
   </si>
   <si>
@@ -969,10 +936,6 @@
     <t>Haitian</t>
   </si>
   <si>
-    <t xml:space="preserve">CID Gallup based the sampling frame on the 2022 projected population figures from the United Nations Economic Commission for Latin America and the Caribbean (ECLAC), acquiring a proportionally stratified sample by region, age, gender, socioeconomic status, and level of urbanization
-</t>
-  </si>
-  <si>
     <t>English and Haitian Creole</t>
   </si>
   <si>
@@ -982,9 +945,6 @@
     <t>Most respondents (73%) reported that they had received up to a middle school diploma, and the remaining 26% of respondents received at least a high school diploma or vocational degree.</t>
   </si>
   <si>
-    <t>Regions and communes were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Within communes, populated areas were selected as the primary sampling unit using probability proportional to size sampling. Enumeration areas were then randomly selected at the neighborhood level. Within the sampled segments, survey administrators performed a systematic random route around a central point of reference to sample households and used the Last Birthday method to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.</t>
-  </si>
-  <si>
     <t>In total, 32 interviewers worked on this project, including 15 female interviewers. Enumerators worked in eight groups of four interviewers with one supervisor each. Interviews were conducted in Haitian Creole.</t>
   </si>
   <si>
@@ -1006,15 +966,6 @@
     <t xml:space="preserve">Most respondents (82%) identified themselves as Afro-Jamaican, followed by Mixed Race (14%).   </t>
   </si>
   <si>
-    <t>Most respondents (77%) reported that they had received at least a high school diploma or  vocational degree and the remaining 19% of respondents received up to a middle school diploma.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regions were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Within cities, parishes were selected as primary sampling units using probability proportional to size sampling. Neighborhoods within the primary sampling units were selected at random, and each house within the selected segment was approached. Within the sampled segments, survey administrators performed a systematic random route to sample households and used a Kish grid to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household. </t>
-  </si>
-  <si>
-    <t>In total, 39 interviewers worked on this project, including 28 female interviewers. Enumerators worked in 19 groups of five interviewers. Interviews were conducted in English.</t>
-  </si>
-  <si>
     <t>The supervisory team directly oversaw or backchecked via telephone 300 interviews (approximately 30% of the total sample). Additional quality control measures included GPS validation, audio quality checks, and checks for abnormal answer patterns. After  quality control, 69 interviews were rejected from the final sample Interviews averaged 40 minutes in length and ranged from 20 to 99 minutes.</t>
   </si>
   <si>
@@ -1024,33 +975,15 @@
     <t>The Bahamas, the Dominican Republic, Guyana, Haiti, and Suriname</t>
   </si>
   <si>
-    <t>Surinamese individual</t>
-  </si>
-  <si>
     <t>Virginia, U.S.A</t>
   </si>
   <si>
-    <t>D3: Designs, Data, Decisions based the sampling frame on 2012 population figures from the General Statistics Bureau of Suriname, acquiring a proportionally stratified sample by region, age, gender, socioeconomic status, and level of urbanization</t>
-  </si>
-  <si>
     <t>English and Dutch</t>
   </si>
   <si>
-    <t xml:space="preserve">One-quarter of all respondents (25%) identified themselves as Maroon, followed by Creole (23%) and Mixed Race (18%). </t>
-  </si>
-  <si>
-    <t>Most respondents (67%) reported that they had received a middle school diploma or less, and the remaining 33% of respondents received at least a high school diploma or vocational degree.</t>
-  </si>
-  <si>
-    <t>Districts were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Due to accessibility issues, the district of Sipaliwini was excluded from the sampling frame. Within districts, communes were selected as the primary sampling unit using probability proportionate to size sampling. Individual sampling segments  were then selected randomly. Within the sampled segments, survey administrators performed a systematic random route to sample households and used survey software to randomly select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.</t>
-  </si>
-  <si>
     <t xml:space="preserve">In total, 19 interviewers worked on this project, including 18 female interviewers. In addition, five fieldwork supervisors and one country lead worked on this project. Interviews were conducted in Dutch. </t>
   </si>
   <si>
-    <t>The supervisory team directly oversaw at least two interviews per interview in the field. During data processing, 80 interviews (approximately 16% of the sample) were selected for audio review by the central office. Additional quality control measures included GPS validation, data checks, and checks for abnormal answer patterns. Interviews averaged 52 minutes in length and ranged from 29 to 84 minutes.</t>
-  </si>
-  <si>
     <t>Data for Suriname, The Bahamas, and Guyana was collected in 2016, 2018, and 2022. Data for the Dominican Republic was collected in 2013, 2016, 2018, and 2022. Data for Haiti was collected in 2021 and 2022. Data for Jamaica was collected in 2011, 2014, 2017, 2019, and 2022</t>
   </si>
   <si>
@@ -1211,6 +1144,85 @@
   </si>
   <si>
     <t xml:space="preserve">Datum Internacional S.A. </t>
+  </si>
+  <si>
+    <t>between July and August 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forty-nine percent (49%) of respondents identified themselves as Afro-Bahamian or “Other,” followed by Indigenous (39%) and Mixed (12%). </t>
+  </si>
+  <si>
+    <t>Most respondents (97%) reported that they had received at least a high school diploma or  vocational degree and the remaining 3% of respondents received up to a middle school diploma.</t>
+  </si>
+  <si>
+    <t>between June and July 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than one-quarter (27%) of all respondents identified themselves as Mestizo, followed by Mulatto (24%) and White (20%). </t>
+  </si>
+  <si>
+    <t>More than half of all respondents (52%) reported that they had received up to a middle school diploma, and the remaining 48% of respondents received at least a high school diploma or vocational degree.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regions and provinces were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Municipalities were then selected as the primary sampling unit using probability proportionate to size sampling. Individual enumeration areas consisted of neighborhood blocks selected via simple random sampling. The number of enumeration areas assigned to each municipality was determined based on the relative population size of each municipality. Within each enumeration area, survey administrators performed a systematic random route to sample households and used the Last Birthday method to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.  </t>
+  </si>
+  <si>
+    <t>Guyanese respondent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thirty percent (39%) of respondents identified themselves as Afro-Guyanese, followed by Mixed Race (26%) and Indo-Guyanese (23%). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than half of all respondents (57%) reported that they received at least a high school diploma or vocational degree and the remaining 43% of respondents received up to a middle school diploma. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regions and metropolitan areas were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Within metropolitan areas, towns and neighborhoods were selected as primary sampling units using probability proportional to size sampling. Street blocks within the primary sampling units were selected at random, and each house within the selected enumeration area was approached. Within each enumeration area, survey administrators performed a systematic random route to sample households and used a Kish grid to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.  </t>
+  </si>
+  <si>
+    <t>The supervisory team directly oversaw or backchecked via telephone 150 interviews (approximately 30% of the total sample). Additional quality control measures included GPS validation, audio quality checks, and checks for abnormal answer patterns. Interviews averaged 41 minutes in length and ranged from 21 to 108 minutes.</t>
+  </si>
+  <si>
+    <t>in June 2022</t>
+  </si>
+  <si>
+    <t>CID Gallup based the sampling frame on the 2022 projected population figures from the Latin American and Caribbean Demographic Center (CELADE) of the United Nations Economic Commission for Latin America and the Caribbean (CEPAL), acquiring a proportionally stratified sample by region, age, gender, socioeconomic status, and level of urbanization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regions, arrondissements, and communes were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Within communes, populated areas were selected as the primary sampling unit using probability proportional to size sampling. Enumeration areas were then randomly selected at the neighborhood level. Within each enumeration area, survey administrators performed a systematic random route around a central point of reference to sample households and used the Last Birthday method to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.  </t>
+  </si>
+  <si>
+    <t>between June and August 2022</t>
+  </si>
+  <si>
+    <t>Most respondents (80%) reported that they received at least a high school diploma or vocational degree and the remaining 20% of respondents received up to a middle school diploma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regions and parishes were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Within parishes, cities were then selected as primary sampling units using probability proportional to size sampling. Neighborhood blocks within the primary sampling units were selected at random, and each house within the selected enumeration area was approached. Within each enumeration area, survey administrators performed a systematic random route to sample households and used a Kish grid to select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.  </t>
+  </si>
+  <si>
+    <t>In total, 39 interviewers worked on this project, including 28 female interviewers. Enumerators worked in groups of five interviewers each. Interviews were conducted in English.</t>
+  </si>
+  <si>
+    <t>between May and June 2022</t>
+  </si>
+  <si>
+    <t>Surinamese respondent</t>
+  </si>
+  <si>
+    <t>D3: Designs, Data, Decisions based the sampling frame on 2012 population figures from the General Statistics Bureau of Suriname, acquiring a proportionally stratified sample by district, age, gender, socioeconomic status, and level of urbanization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One-quarter (25%) of all respondents identified themselves as Maroon, followed by Creole (23%) and Mixed Race (18%). </t>
+  </si>
+  <si>
+    <t>Most respondents (67%) reported that they had received up to a middle school diploma, and the remaining 33% of respondents received at least a high school diploma or vocational degree.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Districts and cities were selected to achieve a nationally representative sample of the country based on population density and geographic coverage. Within cities and towns, communes were selected as the primary sampling unit using probability proportionate to size sampling. Individual enumeration areas were then selected randomly. Within each enumeration area, survey administrators performed a systematic random route to sample households and used survey software to randomly select respondents. If the selected respondent declined to be interviewed or otherwise did not meet the characteristics of the target quota, the interviewer moved on to the next household.  
+Due to accessibility issues, the district of Sipaliwini was excluded from the sampling frame. Within the Brokopondo district, the Brokopondo Centrum and Brownsweg communes were replaced Klaaskreek and Marchallkreek due to flooding that made the original areas inaccessible. </t>
+  </si>
+  <si>
+    <t>The supervisory team directly oversaw at least two interviews per interviewer in the field. During data processing, 80 interviews (approximately 16% of the sample) were selected for audio review by the central office. Additional quality control measures included GPS validation, data checks, and checks for abnormal answer patterns. Interviews averaged 52 minutes in length and ranged from 29 to 104 minutes.</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1489,12 +1501,65 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1821,11 +1886,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A370D2-6729-6642-9050-0182FD4A6CB8}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -1911,7 +1976,7 @@
         <v>1000</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="F2" s="21">
         <v>2022</v>
@@ -1970,7 +2035,7 @@
         <v>1000</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="F3" s="30">
         <v>2022</v>
@@ -2000,7 +2065,7 @@
         <v>123</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="P3" s="22" t="s">
         <v>184</v>
@@ -2088,7 +2153,7 @@
         <v>1029</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>387</v>
+        <v>365</v>
       </c>
       <c r="F5" s="21">
         <v>2022</v>
@@ -2265,7 +2330,7 @@
         <v>1000</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="F8" s="13">
         <v>2021</v>
@@ -2320,7 +2385,7 @@
       <c r="C9" s="21">
         <v>122</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="22">
         <v>500</v>
       </c>
       <c r="E9" s="21" t="s">
@@ -2330,7 +2395,7 @@
         <v>2022</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>20</v>
+        <v>366</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>275</v>
@@ -2348,29 +2413,29 @@
         <v>278</v>
       </c>
       <c r="M9" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="N9" s="40" t="s">
+        <v>368</v>
+      </c>
+      <c r="O9" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="P9" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="Q9" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="R9" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="S9" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="R9" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="S9" s="21" t="s">
-        <v>285</v>
-      </c>
     </row>
     <row r="10" spans="1:23" ht="126" customHeight="1">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="41" t="s">
         <v>162</v>
       </c>
       <c r="B10" s="21">
@@ -2379,57 +2444,57 @@
       <c r="C10" s="21">
         <v>122</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="41">
         <v>1002</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="41" t="s">
         <v>160</v>
       </c>
       <c r="F10" s="21">
         <v>2022</v>
       </c>
-      <c r="G10" s="21">
-        <v>2022</v>
+      <c r="G10" s="21" t="s">
+        <v>369</v>
       </c>
       <c r="H10" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="J10" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="K10" s="21" t="s">
         <v>286</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>288</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>117</v>
       </c>
       <c r="M10" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="N10" s="40" t="s">
+        <v>371</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="P10" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="R10" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="S10" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="O10" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="P10" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q10" s="21" t="s">
-        <v>293</v>
-      </c>
-      <c r="R10" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="S10" s="21" t="s">
-        <v>295</v>
-      </c>
     </row>
     <row r="11" spans="1:23" ht="126" customHeight="1">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="21">
@@ -2438,53 +2503,53 @@
       <c r="C11" s="21">
         <v>122</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="42">
         <v>500</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="22" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="21">
         <v>2022</v>
       </c>
-      <c r="G11" s="21" t="s">
-        <v>296</v>
+      <c r="G11" s="43" t="s">
+        <v>366</v>
       </c>
       <c r="H11" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="I11" s="21" t="s">
-        <v>297</v>
+      <c r="I11" s="22" t="s">
+        <v>373</v>
       </c>
       <c r="J11" s="21" t="s">
         <v>212</v>
       </c>
       <c r="K11" s="21" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="L11" s="21" t="s">
         <v>278</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="N11" s="21" t="s">
-        <v>300</v>
+        <v>374</v>
+      </c>
+      <c r="N11" s="40" t="s">
+        <v>375</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>301</v>
+        <v>376</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>303</v>
+        <v>377</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="S11" s="21" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="126" customHeight="1">
@@ -2497,53 +2562,53 @@
       <c r="C12" s="21">
         <v>122</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="41">
         <v>507</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="41" t="s">
         <v>160</v>
       </c>
       <c r="F12" s="21">
         <v>2022</v>
       </c>
-      <c r="G12" s="21">
-        <v>2022</v>
+      <c r="G12" s="44" t="s">
+        <v>378</v>
       </c>
       <c r="H12" s="21" t="s">
         <v>275</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>306</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>287</v>
+        <v>295</v>
+      </c>
+      <c r="J12" s="41" t="s">
+        <v>285</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>307</v>
+        <v>379</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="N12" s="21" t="s">
-        <v>310</v>
+        <v>297</v>
+      </c>
+      <c r="N12" s="40" t="s">
+        <v>298</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>311</v>
+        <v>380</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="S12" s="21" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="126" customHeight="1">
@@ -2556,63 +2621,64 @@
       <c r="C13" s="21">
         <v>122</v>
       </c>
-      <c r="D13" s="21">
-        <v>531</v>
-      </c>
-      <c r="E13" s="21" t="s">
+      <c r="D13" s="22">
+        <v>1001</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="21">
         <v>2022</v>
       </c>
-      <c r="G13" s="21">
-        <v>2022</v>
+      <c r="G13" s="21" t="s">
+        <v>381</v>
       </c>
       <c r="H13" s="21" t="s">
         <v>275</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>316</v>
-      </c>
-      <c r="J13" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="J13" s="40" t="s">
         <v>212</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="L13" s="21" t="s">
         <v>278</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>318</v>
-      </c>
-      <c r="N13" s="21" t="s">
-        <v>319</v>
+        <v>305</v>
+      </c>
+      <c r="N13" s="40" t="s">
+        <v>382</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>320</v>
+        <v>383</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>321</v>
+        <v>384</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="R13" s="21" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="S13" s="21" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="126" customHeight="1">
       <c r="A14" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="B14" s="21">
-        <v>172</v>
-      </c>
-      <c r="C14" s="21">
+      <c r="B14" s="45">
+        <f>172-5</f>
+        <v>167</v>
+      </c>
+      <c r="C14" s="45">
         <v>122</v>
       </c>
       <c r="D14" s="21">
@@ -2624,65 +2690,110 @@
       <c r="F14" s="21">
         <v>2022</v>
       </c>
-      <c r="G14" s="21">
-        <v>2022</v>
+      <c r="G14" s="21" t="s">
+        <v>385</v>
       </c>
       <c r="H14" s="21" t="s">
         <v>275</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>325</v>
+        <v>386</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>327</v>
+        <v>387</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="M14" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="N14" s="21" t="s">
-        <v>330</v>
+        <v>388</v>
+      </c>
+      <c r="N14" s="40" t="s">
+        <v>389</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>331</v>
+        <v>390</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="Q14" s="21" t="s">
-        <v>333</v>
+        <v>391</v>
       </c>
       <c r="R14" s="21" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="S14" s="21" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" priority="7">
+    <cfRule type="expression" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:K5 A6:XFD1048576 R1:XFD5">
-    <cfRule type="expression" dxfId="1" priority="5">
+  <conditionalFormatting sqref="A1:K5 A6:XFD8 R1:XFD5 A15:XFD1048576 T9:XFD14">
+    <cfRule type="expression" dxfId="6" priority="16">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="17">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:Q5">
+    <cfRule type="expression" dxfId="5" priority="14">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="15">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="expression" priority="11">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O9:S14 K9:M14 A9:I14">
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="10">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:J10 J14 J12">
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="8">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:Q5">
-    <cfRule type="expression" dxfId="0" priority="3">
+  <conditionalFormatting sqref="J13">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9:N14">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2927,7 +3038,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>107</v>
@@ -2942,7 +3053,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>101</v>
@@ -2977,7 +3088,7 @@
         <v>101</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="D19" s="13">
         <v>31</v>
@@ -3006,7 +3117,7 @@
         <v>28</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="D21" s="11">
         <v>26</v>
@@ -3024,7 +3135,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3035,7 +3146,7 @@
         <v>101</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="D23" s="13">
         <v>10</v>
@@ -3064,7 +3175,7 @@
         <v>101</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="D25" s="11">
         <v>15</v>
@@ -3093,7 +3204,7 @@
         <v>101</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="D27" s="13">
         <v>28</v>
@@ -5179,13 +5290,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B147" s="11" t="s">
         <v>96</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="D147" s="11">
         <v>0.78</v>
@@ -5193,13 +5304,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B148" s="11" t="s">
         <v>98</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>340</v>
+        <v>318</v>
       </c>
       <c r="D148" s="11">
         <v>0.16</v>
@@ -5207,13 +5318,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B149" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="D149" s="11">
         <v>0.06</v>
@@ -5221,19 +5332,19 @@
     </row>
     <row r="150" spans="1:4" ht="48">
       <c r="A150" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B150" s="11" t="s">
         <v>142</v>
       </c>
       <c r="C150" s="38" t="s">
-        <v>342</v>
+        <v>320</v>
       </c>
       <c r="D150" s="11"/>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B151" s="11" t="s">
         <v>52</v>
@@ -5247,7 +5358,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B152" s="11" t="s">
         <v>52</v>
@@ -5261,7 +5372,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B153" s="11" t="s">
         <v>55</v>
@@ -5275,7 +5386,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B154" s="11" t="s">
         <v>55</v>
@@ -5289,7 +5400,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B155" s="11" t="s">
         <v>58</v>
@@ -5303,7 +5414,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B156" s="11" t="s">
         <v>58</v>
@@ -5317,7 +5428,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B157" s="11" t="s">
         <v>58</v>
@@ -5331,7 +5442,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B158" s="11" t="s">
         <v>58</v>
@@ -5345,7 +5456,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B159" s="11" t="s">
         <v>58</v>
@@ -5359,7 +5470,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B160" s="11" t="s">
         <v>58</v>
@@ -5373,7 +5484,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B161" s="11" t="s">
         <v>58</v>
@@ -5387,7 +5498,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B162" s="11" t="s">
         <v>58</v>
@@ -5401,7 +5512,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="11" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B163" s="11" t="s">
         <v>58</v>
@@ -5418,10 +5529,10 @@
         <v>162</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
       <c r="D164" s="13">
         <v>0.37</v>
@@ -5432,10 +5543,10 @@
         <v>162</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="C165" s="13" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="D165" s="13">
         <v>0.16</v>
@@ -5446,10 +5557,10 @@
         <v>162</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="D166" s="13">
         <v>0.1</v>
@@ -5460,10 +5571,10 @@
         <v>162</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D167" s="13">
         <v>0.08</v>
@@ -5474,10 +5585,10 @@
         <v>162</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="D168" s="13">
         <v>0.06</v>
@@ -5488,10 +5599,10 @@
         <v>162</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="D169" s="13">
         <v>0.06</v>
@@ -5502,10 +5613,10 @@
         <v>162</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="D170" s="13">
         <v>0.06</v>
@@ -5516,10 +5627,10 @@
         <v>162</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="D171" s="13">
         <v>0.04</v>
@@ -5530,10 +5641,10 @@
         <v>162</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>360</v>
+        <v>338</v>
       </c>
       <c r="D172" s="13">
         <v>0.04</v>
@@ -5544,10 +5655,10 @@
         <v>162</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>361</v>
+        <v>339</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="D173" s="13">
         <v>3.1E-2</v>
@@ -5561,7 +5672,7 @@
         <v>142</v>
       </c>
       <c r="C174" s="21" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -5754,7 +5865,7 @@
         <v>96</v>
       </c>
       <c r="C188" s="11" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
       <c r="D188" s="11">
         <v>0.73</v>
@@ -5768,7 +5879,7 @@
         <v>98</v>
       </c>
       <c r="C189" s="11" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="D189" s="11">
         <v>0.14199999999999999</v>
@@ -5779,10 +5890,10 @@
         <v>163</v>
       </c>
       <c r="B190" s="11" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="C190" s="11" t="s">
-        <v>366</v>
+        <v>344</v>
       </c>
       <c r="D190" s="11">
         <v>0.128</v>
@@ -5796,7 +5907,7 @@
         <v>142</v>
       </c>
       <c r="C191" s="38" t="s">
-        <v>367</v>
+        <v>345</v>
       </c>
       <c r="D191" s="11"/>
     </row>
@@ -5990,7 +6101,7 @@
         <v>96</v>
       </c>
       <c r="C205" s="13" t="s">
-        <v>368</v>
+        <v>346</v>
       </c>
       <c r="D205" s="13">
         <v>0.36899999999999999</v>
@@ -6046,7 +6157,7 @@
         <v>142</v>
       </c>
       <c r="C209" s="21" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -6236,10 +6347,10 @@
         <v>165</v>
       </c>
       <c r="B223" s="11" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
       <c r="C223" s="11" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="D223" s="11">
         <v>0.45800000000000002</v>
@@ -6250,10 +6361,10 @@
         <v>165</v>
       </c>
       <c r="B224" s="11" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="D224" s="11">
         <v>0.31</v>
@@ -6264,10 +6375,10 @@
         <v>165</v>
       </c>
       <c r="B225" s="11" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="C225" s="11" t="s">
-        <v>372</v>
+        <v>350</v>
       </c>
       <c r="D225" s="11">
         <v>0.23</v>
@@ -6281,7 +6392,7 @@
         <v>142</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>373</v>
+        <v>351</v>
       </c>
       <c r="D226" s="11"/>
     </row>
@@ -6475,7 +6586,7 @@
         <v>96</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
       <c r="D240" s="13">
         <v>0.38</v>
@@ -6489,7 +6600,7 @@
         <v>98</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>375</v>
+        <v>353</v>
       </c>
       <c r="D241" s="13">
         <v>0.33</v>
@@ -6503,7 +6614,7 @@
         <v>97</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>376</v>
+        <v>354</v>
       </c>
       <c r="D242" s="13">
         <v>7.0000000000000007E-2</v>
@@ -6517,7 +6628,7 @@
         <v>99</v>
       </c>
       <c r="C243" s="13" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="D243" s="13">
         <v>0.06</v>
@@ -6531,7 +6642,7 @@
         <v>100</v>
       </c>
       <c r="C244" s="13" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
       <c r="D244" s="13">
         <v>0.05</v>
@@ -6545,7 +6656,7 @@
         <v>102</v>
       </c>
       <c r="C245" s="13" t="s">
-        <v>378</v>
+        <v>356</v>
       </c>
       <c r="D245" s="13">
         <v>0.04</v>
@@ -6559,7 +6670,7 @@
         <v>103</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>379</v>
+        <v>357</v>
       </c>
       <c r="D246" s="13">
         <v>0.04</v>
@@ -6573,7 +6684,7 @@
         <v>104</v>
       </c>
       <c r="C247" s="13" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
       <c r="D247" s="13">
         <v>0.03</v>
@@ -6587,7 +6698,7 @@
         <v>105</v>
       </c>
       <c r="C248" s="13" t="s">
-        <v>381</v>
+        <v>359</v>
       </c>
       <c r="D248" s="13">
         <v>0.01</v>
@@ -6601,7 +6712,7 @@
         <v>142</v>
       </c>
       <c r="C249" s="21" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -6795,7 +6906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F8BEAD-D473-7B4F-A0F1-FD90B83F8C12}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -6969,7 +7080,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B9">
         <v>445</v>
@@ -9001,14 +9112,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9255,27 +9364,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9300,9 +9402,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update S03 - S05
</commit_message>
<xml_diff>
--- a/Data/method_summaryData.xlsx
+++ b/Data/method_summaryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiagopardo/Documents/GitHub/LAC-Reports/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63771C7-6638-364D-BDE6-7A1E749F6CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD81F136-49F8-9C4A-962C-98BCEAD89FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling_Frame" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="506">
   <si>
     <t>Sample Size</t>
   </si>
@@ -2014,161 +2014,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="53">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -2696,13 +2542,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A370D2-6729-6642-9050-0182FD4A6CB8}">
-  <dimension ref="A1:W37"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23:S29"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -3542,422 +3388,383 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="192">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:23" ht="256">
+      <c r="A15" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="4">
+        <v>162</v>
+      </c>
+      <c r="C15" s="4">
+        <v>86</v>
+      </c>
+      <c r="D15" s="56">
+        <v>1500</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="57" t="s">
+        <v>440</v>
+      </c>
+      <c r="G15" t="s">
+        <v>502</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="K15" s="58" t="s">
+        <v>443</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="21" t="s">
+        <v>444</v>
+      </c>
+      <c r="O15" s="58" t="s">
+        <v>445</v>
+      </c>
+      <c r="P15" s="58" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>447</v>
+      </c>
+      <c r="R15" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="S15" s="58" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="256">
+      <c r="A16" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="13">
+        <v>115</v>
+      </c>
+      <c r="C16" s="13">
+        <v>77</v>
+      </c>
+      <c r="D16" s="45">
+        <v>1005</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F16" s="57">
+        <v>2022</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="O16" s="44" t="s">
+        <v>454</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="R16" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="S16" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="320">
+      <c r="A17" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="4">
+        <v>162</v>
+      </c>
+      <c r="C17" s="4">
+        <v>86</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="57">
+        <v>2022</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>459</v>
+      </c>
+      <c r="O17" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="P17" s="21" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q17" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="R17" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="S17" s="21" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="272">
+      <c r="A18" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18">
+        <v>162</v>
+      </c>
+      <c r="C18">
+        <v>86</v>
+      </c>
+      <c r="D18" s="54">
+        <v>2002</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>440</v>
+      </c>
+      <c r="G18" t="s">
+        <v>502</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="I18" s="45"/>
+      <c r="J18" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>465</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="O18" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="P18" s="21" t="s">
+        <v>467</v>
+      </c>
+      <c r="Q18" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="R18" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="S18" s="21" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="288">
+      <c r="A19" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="4">
+        <v>162</v>
+      </c>
+      <c r="C19" s="4">
+        <v>86</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" s="57" t="s">
+        <v>440</v>
+      </c>
+      <c r="G19" t="s">
+        <v>502</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>471</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="O19" s="21" t="s">
+        <v>472</v>
+      </c>
+      <c r="P19" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q19" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="R19" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="S19" s="21" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="409.6">
+      <c r="A20" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="13">
+        <v>51</v>
+      </c>
+      <c r="C20" s="13">
+        <v>16</v>
+      </c>
+      <c r="D20" s="45">
+        <v>1014</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="59">
+        <v>2023</v>
+      </c>
+      <c r="G20" s="60" t="s">
+        <v>504</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>476</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>477</v>
+      </c>
+      <c r="O20" s="21" t="s">
+        <v>478</v>
+      </c>
+      <c r="P20" s="21" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>480</v>
+      </c>
+      <c r="R20" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="S20" s="21" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="224">
+      <c r="A21" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="4">
+        <v>162</v>
+      </c>
+      <c r="C21" s="4">
+        <v>86</v>
+      </c>
+      <c r="D21" s="45">
+        <v>2023</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F21" s="57">
+        <v>2022</v>
+      </c>
+      <c r="G21" s="60" t="s">
+        <v>505</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="K21" s="21" t="s">
+        <v>482</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="N21" s="21" t="s">
+        <v>483</v>
+      </c>
+      <c r="O21" s="21" t="s">
+        <v>484</v>
+      </c>
+      <c r="P21" s="21" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q21" s="21" t="s">
+        <v>486</v>
+      </c>
+      <c r="R21" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="S21" s="21" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="192">
+      <c r="A22" s="13" t="s">
         <v>145</v>
-      </c>
-      <c r="B15" s="21">
-        <v>172</v>
-      </c>
-      <c r="C15" s="21">
-        <v>122</v>
-      </c>
-      <c r="D15" s="45">
-        <v>500</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F15" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>387</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K15" s="21" t="s">
-        <v>388</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M15" s="21" t="s">
-        <v>389</v>
-      </c>
-      <c r="N15" s="21" t="s">
-        <v>390</v>
-      </c>
-      <c r="O15" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="P15" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="Q15" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="R15" s="21" t="s">
-        <v>488</v>
-      </c>
-      <c r="S15" s="21" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="192">
-      <c r="A16" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B16" s="21">
-        <v>172</v>
-      </c>
-      <c r="C16" s="21">
-        <v>122</v>
-      </c>
-      <c r="D16" s="2">
-        <v>500</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F16" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M16" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>398</v>
-      </c>
-      <c r="O16" s="21" t="s">
-        <v>399</v>
-      </c>
-      <c r="P16" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="Q16" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="R16" s="21" t="s">
-        <v>489</v>
-      </c>
-      <c r="S16" s="21" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="192">
-      <c r="A17" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="B17" s="21">
-        <v>172</v>
-      </c>
-      <c r="C17" s="21">
-        <v>122</v>
-      </c>
-      <c r="D17" s="54">
-        <v>500</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F17" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I17" s="45" t="s">
-        <v>402</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K17" s="21" t="s">
-        <v>388</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M17" s="21" t="s">
-        <v>403</v>
-      </c>
-      <c r="N17" s="21" t="s">
-        <v>404</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="P17" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="Q17" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="R17" s="21" t="s">
-        <v>491</v>
-      </c>
-      <c r="S17" s="21" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="192">
-      <c r="A18" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" s="21">
-        <v>172</v>
-      </c>
-      <c r="C18" s="21">
-        <v>122</v>
-      </c>
-      <c r="D18" s="54">
-        <v>500</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="J18" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K18" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="N18" s="21" t="s">
-        <v>410</v>
-      </c>
-      <c r="O18" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="P18" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q18" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="R18" s="21" t="s">
-        <v>493</v>
-      </c>
-      <c r="S18" s="21" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="192">
-      <c r="A19" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B19" s="21">
-        <v>172</v>
-      </c>
-      <c r="C19" s="21">
-        <v>122</v>
-      </c>
-      <c r="D19" s="13">
-        <v>500</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F19" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M19" s="21" t="s">
-        <v>416</v>
-      </c>
-      <c r="N19" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="O19" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="P19" s="21" t="s">
-        <v>419</v>
-      </c>
-      <c r="Q19" s="21" t="s">
-        <v>420</v>
-      </c>
-      <c r="R19" s="21" t="s">
-        <v>495</v>
-      </c>
-      <c r="S19" s="21" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="192">
-      <c r="A20" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="21">
-        <v>172</v>
-      </c>
-      <c r="C20" s="21">
-        <v>122</v>
-      </c>
-      <c r="D20" s="13">
-        <v>500</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F20" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="J20" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K20" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M20" s="21" t="s">
-        <v>423</v>
-      </c>
-      <c r="N20" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="O20" s="21" t="s">
-        <v>425</v>
-      </c>
-      <c r="P20" s="21" t="s">
-        <v>426</v>
-      </c>
-      <c r="Q20" s="21" t="s">
-        <v>427</v>
-      </c>
-      <c r="R20" s="21" t="s">
-        <v>496</v>
-      </c>
-      <c r="S20" s="21" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="192">
-      <c r="A21" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B21" s="21">
-        <v>172</v>
-      </c>
-      <c r="C21" s="21">
-        <v>122</v>
-      </c>
-      <c r="D21" s="13">
-        <v>500</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F21" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K21" s="21" t="s">
-        <v>429</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M21" s="21" t="s">
-        <v>430</v>
-      </c>
-      <c r="N21" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="O21" s="21" t="s">
-        <v>431</v>
-      </c>
-      <c r="P21" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q21" s="21" t="s">
-        <v>432</v>
-      </c>
-      <c r="R21" s="21" t="s">
-        <v>498</v>
-      </c>
-      <c r="S21" s="21" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="335">
-      <c r="A22" s="13" t="s">
-        <v>153</v>
       </c>
       <c r="B22" s="21">
         <v>172</v>
@@ -3965,904 +3772,471 @@
       <c r="C22" s="21">
         <v>122</v>
       </c>
-      <c r="D22" s="13">
-        <v>1001</v>
+      <c r="D22" s="45">
+        <v>500</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F22" s="13">
         <v>2022</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>386</v>
       </c>
-      <c r="I22" s="55" t="s">
-        <v>433</v>
-      </c>
-      <c r="J22" s="40" t="s">
-        <v>267</v>
+      <c r="I22" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>434</v>
+        <v>388</v>
       </c>
       <c r="L22" s="13" t="s">
         <v>261</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>435</v>
+        <v>389</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>436</v>
+        <v>390</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>437</v>
+        <v>391</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>438</v>
+        <v>392</v>
       </c>
       <c r="Q22" s="21" t="s">
-        <v>439</v>
+        <v>393</v>
       </c>
       <c r="R22" s="21" t="s">
+        <v>488</v>
+      </c>
+      <c r="S22" s="21" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="192">
+      <c r="A23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="21">
+        <v>172</v>
+      </c>
+      <c r="C23" s="21">
+        <v>122</v>
+      </c>
+      <c r="D23" s="2">
         <v>500</v>
       </c>
-      <c r="S22" s="21" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="256">
-      <c r="A23" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B23" s="4">
-        <v>162</v>
-      </c>
-      <c r="C23" s="4">
-        <v>86</v>
-      </c>
-      <c r="D23" s="56">
-        <v>1500</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F23" s="57" t="s">
-        <v>440</v>
-      </c>
-      <c r="G23" t="s">
-        <v>502</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="K23" s="58" t="s">
-        <v>443</v>
-      </c>
-      <c r="L23" s="4" t="s">
+      <c r="E23" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="13">
+        <v>2022</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="K23" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="L23" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="M23" s="4"/>
+      <c r="M23" s="21" t="s">
+        <v>397</v>
+      </c>
       <c r="N23" s="21" t="s">
-        <v>444</v>
-      </c>
-      <c r="O23" s="58" t="s">
-        <v>445</v>
-      </c>
-      <c r="P23" s="58" t="s">
-        <v>446</v>
+        <v>398</v>
+      </c>
+      <c r="O23" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="P23" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="Q23" s="21" t="s">
-        <v>447</v>
-      </c>
-      <c r="R23" s="44" t="s">
-        <v>448</v>
-      </c>
-      <c r="S23" s="58" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="256">
-      <c r="A24" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" s="13">
-        <v>115</v>
-      </c>
-      <c r="C24" s="13">
-        <v>77</v>
-      </c>
-      <c r="D24" s="45">
-        <v>1005</v>
+        <v>401</v>
+      </c>
+      <c r="R23" s="21" t="s">
+        <v>489</v>
+      </c>
+      <c r="S23" s="21" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="192">
+      <c r="A24" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="21">
+        <v>172</v>
+      </c>
+      <c r="C24" s="21">
+        <v>122</v>
+      </c>
+      <c r="D24" s="54">
+        <v>500</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="F24" s="57">
+        <v>146</v>
+      </c>
+      <c r="F24" s="13">
         <v>2022</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>267</v>
+        <v>386</v>
+      </c>
+      <c r="I24" s="45" t="s">
+        <v>402</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="K24" s="21" t="s">
-        <v>451</v>
+        <v>388</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>452</v>
+        <v>261</v>
+      </c>
+      <c r="M24" s="21" t="s">
+        <v>403</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>453</v>
-      </c>
-      <c r="O24" s="44" t="s">
-        <v>454</v>
+        <v>404</v>
+      </c>
+      <c r="O24" s="21" t="s">
+        <v>405</v>
       </c>
       <c r="P24" s="21" t="s">
-        <v>455</v>
+        <v>400</v>
       </c>
       <c r="Q24" s="21" t="s">
-        <v>456</v>
-      </c>
-      <c r="R24" s="44" t="s">
-        <v>448</v>
+        <v>406</v>
+      </c>
+      <c r="R24" s="21" t="s">
+        <v>491</v>
       </c>
       <c r="S24" s="21" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="320">
-      <c r="A25" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B25" s="4">
-        <v>162</v>
-      </c>
-      <c r="C25" s="4">
-        <v>86</v>
-      </c>
-      <c r="D25" s="2">
-        <v>2010</v>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="192">
+      <c r="A25" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="21">
+        <v>172</v>
+      </c>
+      <c r="C25" s="21">
+        <v>122</v>
+      </c>
+      <c r="D25" s="54">
+        <v>500</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="F25" s="57">
+        <v>146</v>
+      </c>
+      <c r="F25" s="13">
         <v>2022</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>503</v>
+      <c r="G25" s="13" t="s">
+        <v>340</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="13" t="s">
-        <v>267</v>
+        <v>386</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>458</v>
+        <v>408</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>452</v>
+        <v>261</v>
+      </c>
+      <c r="M25" s="21" t="s">
+        <v>409</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>459</v>
+        <v>410</v>
       </c>
       <c r="O25" s="21" t="s">
-        <v>460</v>
+        <v>411</v>
       </c>
       <c r="P25" s="21" t="s">
-        <v>461</v>
+        <v>412</v>
       </c>
       <c r="Q25" s="21" t="s">
-        <v>462</v>
-      </c>
-      <c r="R25" s="44" t="s">
-        <v>448</v>
+        <v>413</v>
+      </c>
+      <c r="R25" s="21" t="s">
+        <v>493</v>
       </c>
       <c r="S25" s="21" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="272">
-      <c r="A26" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="B26">
-        <v>162</v>
-      </c>
-      <c r="C26">
-        <v>86</v>
-      </c>
-      <c r="D26" s="54">
-        <v>2002</v>
-      </c>
-      <c r="E26" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="F26" s="57" t="s">
-        <v>440</v>
-      </c>
-      <c r="G26" t="s">
-        <v>502</v>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="192">
+      <c r="A26" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" s="21">
+        <v>172</v>
+      </c>
+      <c r="C26" s="21">
+        <v>122</v>
+      </c>
+      <c r="D26" s="13">
+        <v>500</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="13">
+        <v>2022</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>340</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="I26" s="45"/>
-      <c r="J26" s="13" t="s">
-        <v>464</v>
+        <v>386</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>465</v>
+        <v>415</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>452</v>
+        <v>261</v>
+      </c>
+      <c r="M26" s="21" t="s">
+        <v>416</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>417</v>
       </c>
       <c r="O26" s="21" t="s">
-        <v>466</v>
+        <v>418</v>
       </c>
       <c r="P26" s="21" t="s">
-        <v>467</v>
+        <v>419</v>
       </c>
       <c r="Q26" s="21" t="s">
-        <v>468</v>
-      </c>
-      <c r="R26" s="44" t="s">
-        <v>448</v>
+        <v>420</v>
+      </c>
+      <c r="R26" s="21" t="s">
+        <v>495</v>
       </c>
       <c r="S26" s="21" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="288">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="192">
       <c r="A27" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B27" s="4">
-        <v>162</v>
-      </c>
-      <c r="C27" s="4">
-        <v>86</v>
-      </c>
-      <c r="D27" s="2">
-        <v>2000</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F27" s="57" t="s">
-        <v>440</v>
-      </c>
-      <c r="G27" t="s">
-        <v>502</v>
+        <v>151</v>
+      </c>
+      <c r="B27" s="21">
+        <v>172</v>
+      </c>
+      <c r="C27" s="21">
+        <v>122</v>
+      </c>
+      <c r="D27" s="13">
+        <v>500</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="13">
+        <v>2022</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>340</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>470</v>
+        <v>386</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>471</v>
+        <v>396</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>452</v>
+        <v>261</v>
+      </c>
+      <c r="M27" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>424</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>472</v>
+        <v>425</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>473</v>
+        <v>426</v>
       </c>
       <c r="Q27" s="21" t="s">
-        <v>474</v>
-      </c>
-      <c r="R27" s="44" t="s">
-        <v>448</v>
+        <v>427</v>
+      </c>
+      <c r="R27" s="21" t="s">
+        <v>496</v>
       </c>
       <c r="S27" s="21" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="409.6">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="192">
       <c r="A28" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="B28" s="13">
-        <v>51</v>
-      </c>
-      <c r="C28" s="13">
-        <v>16</v>
-      </c>
-      <c r="D28" s="45">
-        <v>1014</v>
+        <v>152</v>
+      </c>
+      <c r="B28" s="21">
+        <v>172</v>
+      </c>
+      <c r="C28" s="21">
+        <v>122</v>
+      </c>
+      <c r="D28" s="13">
+        <v>500</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="F28" s="59">
-        <v>2023</v>
-      </c>
-      <c r="G28" s="60" t="s">
-        <v>504</v>
+        <v>146</v>
+      </c>
+      <c r="F28" s="13">
+        <v>2022</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>340</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="J28" s="13" t="s">
-        <v>267</v>
+        <v>386</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>476</v>
+        <v>429</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>452</v>
+        <v>261</v>
+      </c>
+      <c r="M28" s="21" t="s">
+        <v>430</v>
       </c>
       <c r="N28" s="21" t="s">
-        <v>477</v>
+        <v>417</v>
       </c>
       <c r="O28" s="21" t="s">
-        <v>478</v>
+        <v>431</v>
       </c>
       <c r="P28" s="21" t="s">
-        <v>479</v>
+        <v>263</v>
       </c>
       <c r="Q28" s="21" t="s">
-        <v>480</v>
-      </c>
-      <c r="R28" s="44" t="s">
-        <v>448</v>
+        <v>432</v>
+      </c>
+      <c r="R28" s="21" t="s">
+        <v>498</v>
       </c>
       <c r="S28" s="21" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="224">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="335">
       <c r="A29" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" s="4">
-        <v>162</v>
-      </c>
-      <c r="C29" s="4">
-        <v>86</v>
-      </c>
-      <c r="D29" s="45">
-        <v>2023</v>
+        <v>153</v>
+      </c>
+      <c r="B29" s="21">
+        <v>172</v>
+      </c>
+      <c r="C29" s="21">
+        <v>122</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1001</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="F29" s="57">
+      <c r="F29" s="13">
         <v>2022</v>
       </c>
-      <c r="G29" s="60" t="s">
-        <v>505</v>
+      <c r="G29" s="13" t="s">
+        <v>343</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="J29" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="I29" s="55" t="s">
+        <v>433</v>
+      </c>
+      <c r="J29" s="40" t="s">
         <v>267</v>
       </c>
       <c r="K29" s="21" t="s">
-        <v>482</v>
+        <v>434</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>452</v>
+        <v>261</v>
+      </c>
+      <c r="M29" s="21" t="s">
+        <v>435</v>
       </c>
       <c r="N29" s="21" t="s">
-        <v>483</v>
+        <v>436</v>
       </c>
       <c r="O29" s="21" t="s">
-        <v>484</v>
+        <v>437</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>485</v>
+        <v>438</v>
       </c>
       <c r="Q29" s="21" t="s">
-        <v>486</v>
-      </c>
-      <c r="R29" s="44" t="s">
-        <v>448</v>
+        <v>439</v>
+      </c>
+      <c r="R29" s="21" t="s">
+        <v>500</v>
       </c>
       <c r="S29" s="21" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="192">
-      <c r="A30" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30" s="21">
-        <v>172</v>
-      </c>
-      <c r="C30" s="21">
-        <v>122</v>
-      </c>
-      <c r="D30" s="45">
-        <v>500</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F30" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>387</v>
-      </c>
-      <c r="J30" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K30" s="21" t="s">
-        <v>388</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M30" s="21" t="s">
-        <v>389</v>
-      </c>
-      <c r="N30" s="21" t="s">
-        <v>390</v>
-      </c>
-      <c r="O30" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="P30" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="Q30" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="R30" s="21" t="s">
-        <v>488</v>
-      </c>
-      <c r="S30" s="21" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" ht="192">
-      <c r="A31" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B31" s="21">
-        <v>172</v>
-      </c>
-      <c r="C31" s="21">
-        <v>122</v>
-      </c>
-      <c r="D31" s="2">
-        <v>500</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F31" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="J31" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K31" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="L31" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M31" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="N31" s="21" t="s">
-        <v>398</v>
-      </c>
-      <c r="O31" s="21" t="s">
-        <v>399</v>
-      </c>
-      <c r="P31" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="Q31" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="R31" s="21" t="s">
-        <v>489</v>
-      </c>
-      <c r="S31" s="21" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="192">
-      <c r="A32" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="B32" s="21">
-        <v>172</v>
-      </c>
-      <c r="C32" s="21">
-        <v>122</v>
-      </c>
-      <c r="D32" s="54">
-        <v>500</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I32" s="45" t="s">
-        <v>402</v>
-      </c>
-      <c r="J32" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K32" s="21" t="s">
-        <v>388</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M32" s="21" t="s">
-        <v>403</v>
-      </c>
-      <c r="N32" s="21" t="s">
-        <v>404</v>
-      </c>
-      <c r="O32" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="P32" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="Q32" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="R32" s="21" t="s">
-        <v>491</v>
-      </c>
-      <c r="S32" s="21" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" ht="192">
-      <c r="A33" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="B33" s="21">
-        <v>172</v>
-      </c>
-      <c r="C33" s="21">
-        <v>122</v>
-      </c>
-      <c r="D33" s="54">
-        <v>500</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F33" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="J33" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K33" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="L33" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M33" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="N33" s="21" t="s">
-        <v>410</v>
-      </c>
-      <c r="O33" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="P33" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q33" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="R33" s="21" t="s">
-        <v>493</v>
-      </c>
-      <c r="S33" s="21" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="192">
-      <c r="A34" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B34" s="21">
-        <v>172</v>
-      </c>
-      <c r="C34" s="21">
-        <v>122</v>
-      </c>
-      <c r="D34" s="13">
-        <v>500</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F34" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="J34" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K34" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M34" s="21" t="s">
-        <v>416</v>
-      </c>
-      <c r="N34" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="O34" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="P34" s="21" t="s">
-        <v>419</v>
-      </c>
-      <c r="Q34" s="21" t="s">
-        <v>420</v>
-      </c>
-      <c r="R34" s="21" t="s">
-        <v>495</v>
-      </c>
-      <c r="S34" s="21" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="192">
-      <c r="A35" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B35" s="21">
-        <v>172</v>
-      </c>
-      <c r="C35" s="21">
-        <v>122</v>
-      </c>
-      <c r="D35" s="13">
-        <v>500</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F35" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I35" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="J35" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K35" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="L35" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M35" s="21" t="s">
-        <v>423</v>
-      </c>
-      <c r="N35" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="O35" s="21" t="s">
-        <v>425</v>
-      </c>
-      <c r="P35" s="21" t="s">
-        <v>426</v>
-      </c>
-      <c r="Q35" s="21" t="s">
-        <v>427</v>
-      </c>
-      <c r="R35" s="21" t="s">
-        <v>496</v>
-      </c>
-      <c r="S35" s="21" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="192">
-      <c r="A36" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B36" s="21">
-        <v>172</v>
-      </c>
-      <c r="C36" s="21">
-        <v>122</v>
-      </c>
-      <c r="D36" s="13">
-        <v>500</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F36" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="J36" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="K36" s="21" t="s">
-        <v>429</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M36" s="21" t="s">
-        <v>430</v>
-      </c>
-      <c r="N36" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="O36" s="21" t="s">
-        <v>431</v>
-      </c>
-      <c r="P36" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q36" s="21" t="s">
-        <v>432</v>
-      </c>
-      <c r="R36" s="21" t="s">
-        <v>498</v>
-      </c>
-      <c r="S36" s="21" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="335">
-      <c r="A37" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B37" s="21">
-        <v>172</v>
-      </c>
-      <c r="C37" s="21">
-        <v>122</v>
-      </c>
-      <c r="D37" s="13">
-        <v>1001</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="F37" s="13">
-        <v>2022</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I37" s="55" t="s">
-        <v>433</v>
-      </c>
-      <c r="J37" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="K37" s="21" t="s">
-        <v>434</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="M37" s="21" t="s">
-        <v>435</v>
-      </c>
-      <c r="N37" s="21" t="s">
-        <v>436</v>
-      </c>
-      <c r="O37" s="21" t="s">
-        <v>437</v>
-      </c>
-      <c r="P37" s="21" t="s">
-        <v>438</v>
-      </c>
-      <c r="Q37" s="21" t="s">
-        <v>439</v>
-      </c>
-      <c r="R37" s="21" t="s">
-        <v>500</v>
-      </c>
-      <c r="S37" s="21" t="s">
         <v>501</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:K1 R1:XFD1 A38:XFD1048576 T2:XFD37">
-    <cfRule type="expression" dxfId="52" priority="171">
+  <conditionalFormatting sqref="A1:K1 R1:XFD1 A30:XFD1048576 T2:XFD29">
+    <cfRule type="expression" dxfId="30" priority="171">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="172">
@@ -4870,7 +4244,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:Q1">
-    <cfRule type="expression" dxfId="51" priority="169">
+    <cfRule type="expression" dxfId="29" priority="169">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="170">
@@ -4883,7 +4257,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:S5">
-    <cfRule type="expression" dxfId="50" priority="136">
+    <cfRule type="expression" dxfId="28" priority="136">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="137">
@@ -4896,7 +4270,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:S8">
-    <cfRule type="expression" dxfId="49" priority="133">
+    <cfRule type="expression" dxfId="27" priority="133">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="134">
@@ -4909,7 +4283,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:M14 A9:I14 O9:S14">
-    <cfRule type="expression" dxfId="48" priority="130">
+    <cfRule type="expression" dxfId="26" priority="130">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="131">
@@ -4917,7 +4291,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:J10 J14 J12">
-    <cfRule type="expression" dxfId="47" priority="128">
+    <cfRule type="expression" dxfId="25" priority="128">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="129">
@@ -4925,7 +4299,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="expression" dxfId="46" priority="126">
+    <cfRule type="expression" dxfId="24" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="127">
@@ -4933,7 +4307,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="45" priority="124">
+    <cfRule type="expression" dxfId="23" priority="124">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="125">
@@ -4941,136 +4315,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:N14">
-    <cfRule type="expression" dxfId="44" priority="122">
+    <cfRule type="expression" dxfId="22" priority="122">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="123">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" priority="75">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:A22 K16:Q16 I15:I21 K15:M15 O15:S15 K17:M17 O17:Q17 K18:Q18 K19:M19 O19:Q19 K20:Q20 K21:M21 O21:Q21 K22:Q22 D15:H22 R16:S22">
-    <cfRule type="expression" dxfId="35" priority="73">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="74">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C22">
-    <cfRule type="expression" dxfId="34" priority="71">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="72">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
-    <cfRule type="expression" dxfId="33" priority="69">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="70">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J16">
-    <cfRule type="expression" dxfId="32" priority="67">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="68">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
-    <cfRule type="expression" dxfId="31" priority="65">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="66">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="expression" dxfId="30" priority="63">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="64">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J19">
-    <cfRule type="expression" dxfId="29" priority="61">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="62">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J20">
-    <cfRule type="expression" dxfId="28" priority="59">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="60">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21">
-    <cfRule type="expression" dxfId="27" priority="57">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="58">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22">
-    <cfRule type="expression" dxfId="26" priority="55">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="56">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N15">
-    <cfRule type="expression" dxfId="25" priority="53">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="54">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N17">
-    <cfRule type="expression" dxfId="24" priority="51">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="52">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N19">
-    <cfRule type="expression" dxfId="23" priority="49">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="50">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N21">
-    <cfRule type="expression" dxfId="22" priority="47">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="48">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D23">
     <cfRule type="expression" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30:A37 K31:Q31 I30:I36 K30:M30 O30:S30 K32:M32 O32:Q32 K33:Q33 K34:M34 O34:Q34 K35:Q35 K36:M36 O36:Q36 K37:Q37 D30:H37 R31:S37">
+  <conditionalFormatting sqref="A22:A29 K23:Q23 I22:I28 K22:M22 O22:S22 K24:M24 O24:Q24 K25:Q25 K26:M26 O26:Q26 K27:Q27 K28:M28 O28:Q28 K29:Q29 D22:H29 R23:S29">
     <cfRule type="expression" dxfId="21" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5078,7 +4335,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C37">
+  <conditionalFormatting sqref="B22:C29">
     <cfRule type="expression" dxfId="20" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5086,7 +4343,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J30">
+  <conditionalFormatting sqref="J22">
     <cfRule type="expression" dxfId="19" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5094,7 +4351,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
+  <conditionalFormatting sqref="J23">
     <cfRule type="expression" dxfId="18" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5102,7 +4359,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
+  <conditionalFormatting sqref="J24">
     <cfRule type="expression" dxfId="17" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5110,7 +4367,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33">
+  <conditionalFormatting sqref="J25">
     <cfRule type="expression" dxfId="16" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5118,7 +4375,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
+  <conditionalFormatting sqref="J26">
     <cfRule type="expression" dxfId="15" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5126,7 +4383,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
+  <conditionalFormatting sqref="J27">
     <cfRule type="expression" dxfId="14" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5134,7 +4391,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36">
+  <conditionalFormatting sqref="J28">
     <cfRule type="expression" dxfId="13" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5142,7 +4399,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J37">
+  <conditionalFormatting sqref="J29">
     <cfRule type="expression" dxfId="12" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5150,7 +4407,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30">
+  <conditionalFormatting sqref="N22">
     <cfRule type="expression" dxfId="11" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5158,7 +4415,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N32">
+  <conditionalFormatting sqref="N24">
     <cfRule type="expression" dxfId="10" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5166,7 +4423,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N34">
+  <conditionalFormatting sqref="N26">
     <cfRule type="expression" dxfId="9" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5174,7 +4431,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N36">
+  <conditionalFormatting sqref="N28">
     <cfRule type="expression" dxfId="8" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5182,12 +4439,12 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
+  <conditionalFormatting sqref="D17">
     <cfRule type="expression" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A29 D24:E24 G24:N24 S24:S29 P24:Q24 D25:Q29 D23:I23">
+  <conditionalFormatting sqref="A15:A21 D16:E16 G16:N16 S16:S21 P16:Q16 D17:Q21 D15:I15">
     <cfRule type="expression" dxfId="7" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5195,7 +4452,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23:M23 S23 O23:P23">
+  <conditionalFormatting sqref="K15:M15 S15 O15:P15">
     <cfRule type="expression" dxfId="6" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5203,7 +4460,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:C29">
+  <conditionalFormatting sqref="B15:C21">
     <cfRule type="expression" dxfId="5" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5211,7 +4468,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J23">
+  <conditionalFormatting sqref="J15">
     <cfRule type="expression" dxfId="4" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5219,7 +4476,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q23">
+  <conditionalFormatting sqref="Q15">
     <cfRule type="expression" dxfId="3" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5227,7 +4484,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O24">
+  <conditionalFormatting sqref="O16">
     <cfRule type="expression" dxfId="2" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5235,7 +4492,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N23">
+  <conditionalFormatting sqref="N15">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -5243,7 +4500,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R23:R29">
+  <conditionalFormatting sqref="R15:R21">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -11566,12 +10823,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11818,20 +11077,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11856,18 +11122,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>